<commit_message>
Clauses CREATE & UNWIND.
</commit_message>
<xml_diff>
--- a/test/Templates.xlsx
+++ b/test/Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="24" windowWidth="5910" windowHeight="4980"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="5910" windowHeight="4980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,24 +429,15 @@
     <t>SHORTESTPATH ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
   </si>
   <si>
-    <t>ALLSHORTESTPATH ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
-  </si>
-  <si>
     <t>anonymous_pattern_part</t>
   </si>
   <si>
     <t>pattern_part</t>
   </si>
   <si>
-    <t>variable_1 = ALLSHORTESTPATH ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
-  </si>
-  <si>
     <t>pattern</t>
   </si>
   <si>
-    <t>variable_1 = ALLSHORTESTPATH ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) ) , variable_1 = ALLSHORTESTPATH ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
-  </si>
-  <si>
     <t>where</t>
   </si>
   <si>
@@ -537,9 +528,6 @@
     <t>nOt + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 = + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 aNd nOt + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 = + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 xOr nOt + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 = + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 aNd nOt + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 = + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 oR nOt + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 = + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 aNd nOt + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 = + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 xOr nOt + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 = + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 aNd nOt + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 = + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 - + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1</t>
   </si>
   <si>
-    <t>=B24</t>
-  </si>
-  <si>
     <t>WHEN - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 THEN - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1</t>
   </si>
   <si>
@@ -631,6 +619,18 @@
   </si>
   <si>
     <t>= nOt 'test_1' .property_1 :label_1 is null oR 'test_1' .property_1 :label_1 is null</t>
+  </si>
+  <si>
+    <t>variable_1 = ALLSHORTESTPATHS ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
+  </si>
+  <si>
+    <t>variable_1 = ALLSHORTESTPATHS ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) ) , variable_1 = ALLSHORTESTPATHS ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
+  </si>
+  <si>
+    <t>ALLSHORTESTPATHS ( ( variable_1 :node_1 { parameter_1 } ) &lt;-- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] --&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1</t>
   </si>
 </sst>
 </file>
@@ -999,18 +999,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7890625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="151.7890625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.83984375" style="2"/>
+    <col min="1" max="1" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="151.85546875" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1018,143 +1018,143 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="109.2" x14ac:dyDescent="0.6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="126" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>51</v>
       </c>
@@ -1202,15 +1202,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1218,143 +1218,143 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="327.9" x14ac:dyDescent="0.65">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="378.75" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="48" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="93.9" x14ac:dyDescent="0.65">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="95.25" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="171.9" x14ac:dyDescent="0.65">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="189.75" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="171.9" x14ac:dyDescent="0.65">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="189.75" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>72</v>
       </c>
@@ -1362,23 +1362,23 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>72</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>70</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>18</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="50" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>53</v>
       </c>
@@ -1410,47 +1410,47 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="51" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B51" s="4" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A52" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A54" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>94</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="57" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>45</v>
       </c>
@@ -1466,23 +1466,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="58" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>30</v>
       </c>
@@ -1490,23 +1490,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.6">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>102</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="64" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>104</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>104</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="66" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>78</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>78</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>78</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>78</v>
       </c>
@@ -1570,39 +1570,39 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="71" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.6">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.6">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.6">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>32</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>32</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="77" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>13</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="78" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>49</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>27</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>27</v>
       </c>
@@ -1650,87 +1650,87 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="81" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.6">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.6">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.6">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.6">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.6">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B88" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
-      <c r="A89" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="A90" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="91" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>131</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>131</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="93" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>131</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="94" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>121</v>
       </c>
@@ -1762,23 +1762,23 @@
         <v>122</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="95" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="96" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>110</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>110</v>
       </c>
@@ -1794,47 +1794,47 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="99" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.6">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.6">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>23</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="105" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>65</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>65</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>65</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="108" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>97</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>97</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>97</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>97</v>
       </c>
@@ -1898,15 +1898,15 @@
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
+    <row r="112" spans="1:2" ht="48" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>35</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>35</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>35</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>35</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="117" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>109</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="118" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>93</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="119" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>111</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>111</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>111</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>111</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>111</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>111</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="125" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>118</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>118</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="127" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>106</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>106</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="129" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>77</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="130" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>77</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="131" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>77</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="132" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>44</v>
       </c>
@@ -2066,15 +2066,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="133" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>135</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>135</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="135" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>21</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>21</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>21</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="138" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>58</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>58</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="140" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>6</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>6</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>6</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="143" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>10</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>10</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="145" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>20</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>20</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>20</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="148" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>2</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>2</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>2</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>2</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="152" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>61</v>
       </c>
@@ -2226,12 +2226,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="153" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2240,7 +2240,7 @@
     <sortCondition ref="B2:B153"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2250,7 +2250,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2262,7 +2262,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Clauses REMOVE, RETURN, SET & WITH.
</commit_message>
<xml_diff>
--- a/test/Templates.xlsx
+++ b/test/Templates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="417">
   <si>
     <t>LHS</t>
   </si>
@@ -1036,6 +1036,237 @@
   </si>
   <si>
     <t>variable_1 = RELATIONSHIP : symbolic_1 ( symbolic_2 = \"test string\" )</t>
+  </si>
+  <si>
+    <t>remove_item</t>
+  </si>
+  <si>
+    <t>sort_item</t>
+  </si>
+  <si>
+    <t>test' .property_1 .property2? :label_1 :label_2 .property_3 .property4?</t>
+  </si>
+  <si>
+    <t>test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASCENDING</t>
+  </si>
+  <si>
+    <t>test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASCENDING</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 DESCENDING</t>
+  </si>
+  <si>
+    <t>test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? DESCENDING</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 DESC</t>
+  </si>
+  <si>
+    <t>test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? DESC</t>
+  </si>
+  <si>
+    <t>LIMIT 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4?</t>
+  </si>
+  <si>
+    <t>LIMIT - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>SKIP - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>SKIP 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4?</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC</t>
+  </si>
+  <si>
+    <t>ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASCENDING</t>
+  </si>
+  <si>
+    <t>ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 DESC</t>
+  </si>
+  <si>
+    <t>ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 DESCENDING</t>
+  </si>
+  <si>
+    <t>ORDER BY 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4?</t>
+  </si>
+  <si>
+    <t>ORDER BY 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>ORDER BY 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASCENDING</t>
+  </si>
+  <si>
+    <t>return_item</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1</t>
+  </si>
+  <si>
+    <t>test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? AS variable_1</t>
+  </si>
+  <si>
+    <t>return_items</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>* , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4?</t>
+  </si>
+  <si>
+    <t>* , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1</t>
+  </si>
+  <si>
+    <t>* , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? AS variable_1</t>
+  </si>
+  <si>
+    <t>* , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1</t>
+  </si>
+  <si>
+    <t>return_body</t>
+  </si>
+  <si>
+    <t>ORDER BY + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 ASC</t>
+  </si>
+  <si>
+    <t>ORDER BY + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 ASCENDING</t>
+  </si>
+  <si>
+    <t>ORDER BY + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 DESCENDING</t>
+  </si>
+  <si>
+    <t>ORDER BY + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 DESC</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 AS variable_1</t>
+  </si>
+  <si>
+    <t>* , + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 AS variable_1</t>
+  </si>
+  <si>
+    <t>SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 ASC</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 ASCENDING</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 DESCENDING</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 DESC</t>
+  </si>
+  <si>
+    <t>LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>ORDER BY + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>ORDER BY 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? DESC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>ORDER BY 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? DESCENDING , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>* , + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 AS variable_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>* , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 AS variable_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>- 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? AS variable_1 SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 , - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 AS variable_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>+ 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 ORDER BY - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ASC , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? ASC SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
+  </si>
+  <si>
+    <t>* , 'test' .property_1 .property2? :label_1 :label_2 .property_3 .property4? AS variable_1 SKIP + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1 LIMIT + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 % + 'test_1' .property_1 :label_1 conTains 'test_2' .property_1 :label_1 ^ - 'test_1' .property_1 :label_1 contains 'test_2' .property_1 :label_1</t>
   </si>
 </sst>
 </file>
@@ -1412,17 +1643,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B314"/>
+  <dimension ref="A1:B432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="B265" sqref="B265:B300"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="151.85546875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="37.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="151.83984375" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.83984375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
@@ -1481,7 +1712,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1489,7 +1720,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1497,7 +1728,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
       <c r="A10" s="7" t="s">
         <v>63</v>
       </c>
@@ -1505,7 +1736,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="63.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
       <c r="A11" s="5" t="s">
         <v>64</v>
       </c>
@@ -1513,7 +1744,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -1521,7 +1752,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
@@ -1529,7 +1760,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
@@ -1537,7 +1768,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1545,7 +1776,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -1553,7 +1784,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -1561,7 +1792,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -1569,7 +1800,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -1577,7 +1808,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -1585,7 +1816,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A21" s="7" t="s">
         <v>40</v>
       </c>
@@ -1593,7 +1824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -1601,7 +1832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1609,7 +1840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A24" s="7" t="s">
         <v>51</v>
       </c>
@@ -1617,7 +1848,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A25" s="7" t="s">
         <v>33</v>
       </c>
@@ -1625,7 +1856,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1633,7 +1864,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A27" s="7" t="s">
         <v>34</v>
       </c>
@@ -1641,7 +1872,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
       <c r="A28" s="7" t="s">
         <v>92</v>
       </c>
@@ -1649,7 +1880,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="378.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="327.9" x14ac:dyDescent="0.65">
       <c r="A29" s="7" t="s">
         <v>89</v>
       </c>
@@ -1657,7 +1888,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
       <c r="A30" s="7" t="s">
         <v>90</v>
       </c>
@@ -1665,7 +1896,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
       <c r="A31" s="7" t="s">
         <v>91</v>
       </c>
@@ -1673,7 +1904,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A32" s="7" t="s">
         <v>158</v>
       </c>
@@ -1681,7 +1912,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
       <c r="A33" s="7" t="s">
         <v>82</v>
       </c>
@@ -1689,7 +1920,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A34" s="7" t="s">
         <v>83</v>
       </c>
@@ -1697,7 +1928,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
       <c r="A35" s="7" t="s">
         <v>84</v>
       </c>
@@ -1705,7 +1936,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="48" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
       <c r="A36" s="7" t="s">
         <v>85</v>
       </c>
@@ -1713,7 +1944,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="95.25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="93.9" x14ac:dyDescent="0.65">
       <c r="A37" s="7" t="s">
         <v>86</v>
       </c>
@@ -1721,7 +1952,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="189.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="171.9" x14ac:dyDescent="0.65">
       <c r="A38" s="7" t="s">
         <v>87</v>
       </c>
@@ -1729,7 +1960,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="189.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="171.9" x14ac:dyDescent="0.65">
       <c r="A39" s="7" t="s">
         <v>88</v>
       </c>
@@ -1737,7 +1968,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A40" s="7" t="s">
         <v>76</v>
       </c>
@@ -1745,7 +1976,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A41" s="2" t="s">
         <v>76</v>
       </c>
@@ -1753,7 +1984,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A42" s="7" t="s">
         <v>72</v>
       </c>
@@ -1761,7 +1992,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
@@ -1769,7 +2000,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A44" s="2" t="s">
         <v>72</v>
       </c>
@@ -1777,7 +2008,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A45" s="2" t="s">
         <v>72</v>
       </c>
@@ -1785,7 +2016,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
@@ -1793,7 +2024,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A47" s="2" t="s">
         <v>72</v>
       </c>
@@ -1801,7 +2032,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A48" s="7" t="s">
         <v>70</v>
       </c>
@@ -1809,7 +2040,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A49" s="7" t="s">
         <v>18</v>
       </c>
@@ -1817,7 +2048,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A50" s="7" t="s">
         <v>53</v>
       </c>
@@ -1825,7 +2056,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A51" s="7" t="s">
         <v>141</v>
       </c>
@@ -1833,7 +2064,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A52" s="2" t="s">
         <v>141</v>
       </c>
@@ -1841,7 +2072,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A53" s="2" t="s">
         <v>141</v>
       </c>
@@ -1849,7 +2080,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A54" s="2" t="s">
         <v>141</v>
       </c>
@@ -1857,7 +2088,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A55" s="7" t="s">
         <v>75</v>
       </c>
@@ -1865,7 +2096,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A56" s="7" t="s">
         <v>206</v>
       </c>
@@ -1873,7 +2104,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A57" s="2" t="s">
         <v>206</v>
       </c>
@@ -1881,7 +2112,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A58" s="2" t="s">
         <v>206</v>
       </c>
@@ -1889,7 +2120,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A59" s="2" t="s">
         <v>206</v>
       </c>
@@ -1897,7 +2128,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A60" s="2" t="s">
         <v>206</v>
       </c>
@@ -1905,7 +2136,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A61" s="2" t="s">
         <v>206</v>
       </c>
@@ -1913,7 +2144,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A62" s="7" t="s">
         <v>218</v>
       </c>
@@ -1921,7 +2152,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A63" s="2" t="s">
         <v>218</v>
       </c>
@@ -1929,7 +2160,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A64" s="2" t="s">
         <v>218</v>
       </c>
@@ -1937,7 +2168,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A65" s="2" t="s">
         <v>218</v>
       </c>
@@ -1945,7 +2176,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A66" s="2" t="s">
         <v>218</v>
       </c>
@@ -1953,7 +2184,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A67" s="7" t="s">
         <v>212</v>
       </c>
@@ -1961,7 +2192,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A68" s="2" t="s">
         <v>212</v>
       </c>
@@ -1969,7 +2200,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A69" s="2" t="s">
         <v>212</v>
       </c>
@@ -1977,7 +2208,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A70" s="2" t="s">
         <v>212</v>
       </c>
@@ -1985,7 +2216,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A71" s="2" t="s">
         <v>212</v>
       </c>
@@ -1993,7 +2224,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A72" s="7" t="s">
         <v>94</v>
       </c>
@@ -2001,7 +2232,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A73" s="7" t="s">
         <v>45</v>
       </c>
@@ -2009,1938 +2240,2806 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
       <c r="A74" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A75" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A76" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+      <c r="A77" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="78" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A78" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A76" s="7" t="s">
+    <row r="79" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A79" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A80" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A81" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A79" s="7" t="s">
+    <row r="82" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A82" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A83" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A84" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A85" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A86" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A87" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A88" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A89" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A90" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A91" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A92" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A93" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A94" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A95" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A96" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A97" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A98" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A99" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A100" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A101" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A102" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A103" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A104" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A105" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A106" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A107" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A108" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A109" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A110" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A111" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A112" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A113" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A114" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B114" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A115" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A116" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A117" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B117" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A115" s="7" t="s">
+    <row r="118" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A118" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="119" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A119" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A120" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A118" s="7" t="s">
+    <row r="121" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+      <c r="A121" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A122" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A123" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A124" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A125" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A126" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A127" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A128" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A129" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A130" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A131" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A132" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A133" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A134" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A135" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B135" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A136" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A137" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A138" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B138" s="4" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A136" s="7" t="s">
+    <row r="139" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A139" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B139" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A137" s="7" t="s">
+    <row r="140" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A140" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A141" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A139" s="7" t="s">
+    <row r="142" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A142" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A143" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A144" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A145" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A146" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A147" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A148" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A149" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A150" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A151" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A152" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A153" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A154" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B154" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A155" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A156" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A157" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B157" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A155" s="7" t="s">
+    <row r="158" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A158" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B157" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A159" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B159" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A160" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A161" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A162" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B162" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A160" s="7" t="s">
+    <row r="163" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A163" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A164" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A165" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B165" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A166" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A167" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A168" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B168" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A166" s="7" t="s">
+    <row r="169" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A169" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A167" s="7" t="s">
+    <row r="170" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A170" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A168" s="7" t="s">
+    <row r="171" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A171" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A172" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A173" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A174" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A175" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A176" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A177" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A178" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A179" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A180" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A181" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A182" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B182" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A183" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A184" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A185" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A186" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B186" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A187" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B187" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="2" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A188" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B188" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A170" s="7" t="s">
+    <row r="189" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A189" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B189" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A171" s="7" t="s">
+    <row r="190" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A190" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B190" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A191" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B191" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A192" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B192" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="2" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A193" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B193" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A194" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B194" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A195" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B195" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="s">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A196" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B196" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A178" s="7" t="s">
+    <row r="197" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+      <c r="A197" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B197" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A179" s="2" t="s">
+    <row r="198" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A198" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B198" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A180" s="7" t="s">
+    <row r="199" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+      <c r="A199" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B180" s="4" t="s">
+      <c r="B199" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A200" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B200" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A182" s="2" t="s">
+    <row r="201" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A201" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B201" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A183" s="7" t="s">
+    <row r="202" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+      <c r="A202" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B202" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A184" s="7" t="s">
+    <row r="203" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+      <c r="A203" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B203" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
+    <row r="204" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A204" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B204" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A186" s="7" t="s">
+    <row r="205" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A205" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B205" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A206" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B206" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
+    <row r="207" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A207" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B207" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A208" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="B208" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A190" s="7" t="s">
+    <row r="209" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A209" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B209" s="4" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A210" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B210" s="4" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A211" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B192" s="4" t="s">
+      <c r="B211" s="4" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A193" s="7" t="s">
+    <row r="212" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A212" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B212" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A194" s="7" t="s">
+    <row r="213" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A213" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B213" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="2" t="s">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A214" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B214" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="2" t="s">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A215" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="B215" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A197" s="7" t="s">
+    <row r="216" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A216" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B216" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A217" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B198" s="4" t="s">
+      <c r="B217" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A218" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B218" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A219" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="B219" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="48" x14ac:dyDescent="0.3">
-      <c r="A201" s="7" t="s">
+    <row r="220" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
+      <c r="A220" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="B220" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A202" s="7" t="s">
+    <row r="221" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A221" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B202" s="4" t="s">
+      <c r="B221" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="2" t="s">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A222" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B203" s="4" t="s">
+      <c r="B222" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="2" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A223" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B204" s="4" t="s">
+      <c r="B223" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="2" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A224" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="B224" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A206" s="7" t="s">
+    <row r="225" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A225" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B206" s="4" t="s">
+      <c r="B225" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A207" s="7" t="s">
+    <row r="226" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A226" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B207" s="4" t="s">
+      <c r="B226" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A208" s="7" t="s">
+    <row r="227" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A227" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B208" s="4" t="s">
+      <c r="B227" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A228" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B209" s="4" t="s">
+      <c r="B228" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A229" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B210" s="4" t="s">
+      <c r="B229" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A230" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B211" s="4" t="s">
+      <c r="B230" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A231" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B212" s="4" t="s">
+      <c r="B231" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="2" t="s">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A232" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B213" s="4" t="s">
+      <c r="B232" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A214" s="7" t="s">
+    <row r="233" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A233" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B214" s="4" t="s">
+      <c r="B233" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A234" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B215" s="4" t="s">
+      <c r="B234" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="2" t="s">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A235" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B216" s="4" t="s">
+      <c r="B235" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="2" t="s">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A236" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B217" s="4" t="s">
+      <c r="B236" s="4" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="2" t="s">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A237" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B218" s="4" t="s">
+      <c r="B237" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="2" t="s">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A238" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B219" s="4" t="s">
+      <c r="B238" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="2" t="s">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A239" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B220" s="4" t="s">
+      <c r="B239" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="2" t="s">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A240" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B221" s="4" t="s">
+      <c r="B240" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="2" t="s">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A241" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B222" s="4" t="s">
+      <c r="B241" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A242" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B223" s="4" t="s">
+      <c r="B242" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="2" t="s">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A243" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B224" s="4" t="s">
+      <c r="B243" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="2" t="s">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A244" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B225" s="4" t="s">
+      <c r="B244" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="2" t="s">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A245" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B226" s="4" t="s">
+      <c r="B245" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="2" t="s">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A246" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B227" s="4" t="s">
+      <c r="B246" s="4" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A247" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B228" s="4" t="s">
+      <c r="B247" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="2" t="s">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A248" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B229" s="4" t="s">
+      <c r="B248" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A249" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B230" s="4" t="s">
+      <c r="B249" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="2" t="s">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A250" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B231" s="4" t="s">
+      <c r="B250" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="2" t="s">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A251" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B232" s="4" t="s">
+      <c r="B251" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A252" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B233" s="4" t="s">
+      <c r="B252" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A234" s="7" t="s">
+    <row r="253" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A253" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B234" s="4" t="s">
+      <c r="B253" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="2" t="s">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A254" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B235" s="4" t="s">
+      <c r="B254" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A236" s="7" t="s">
+    <row r="255" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A255" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B236" s="4" t="s">
+      <c r="B255" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A256" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B237" s="4" t="s">
+      <c r="B256" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A238" s="7" t="s">
+    <row r="257" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A257" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B238" s="4" t="s">
+      <c r="B257" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A239" s="2" t="s">
+    <row r="258" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A258" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B239" s="4" t="s">
+      <c r="B258" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A240" s="2" t="s">
+    <row r="259" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A259" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B240" s="4" t="s">
+      <c r="B259" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A241" s="7" t="s">
+    <row r="260" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A260" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B260" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A261" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B261" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A262" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B262" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A263" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B263" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A264" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A265" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B265" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A266" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B266" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A267" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B267" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A268" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B268" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A269" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B269" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="78" x14ac:dyDescent="0.6">
+      <c r="A270" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B270" s="4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A271" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B271" s="4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A272" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B272" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A273" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B273" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A274" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A275" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B275" s="4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="171.6" x14ac:dyDescent="0.6">
+      <c r="A276" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B276" s="4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="78" x14ac:dyDescent="0.6">
+      <c r="A277" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B277" s="4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="124.8" x14ac:dyDescent="0.6">
+      <c r="A278" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B278" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A279" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B279" s="4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A280" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B280" s="4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A281" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="78" x14ac:dyDescent="0.6">
+      <c r="A282" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B282" s="4" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="156" x14ac:dyDescent="0.6">
+      <c r="A283" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B283" s="4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A284" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A285" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B285" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A286" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B286" s="6" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A287" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B287" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A288" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B288" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A289" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B289" s="6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A290" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B290" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="109.2" x14ac:dyDescent="0.6">
+      <c r="A291" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B291" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A292" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B292" s="4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A293" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B293" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="109.2" x14ac:dyDescent="0.6">
+      <c r="A294" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B294" s="4" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="78" x14ac:dyDescent="0.6">
+      <c r="A295" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B295" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="156" x14ac:dyDescent="0.6">
+      <c r="A296" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B296" s="4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A297" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B297" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A298" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B298" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A299" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B299" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A300" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B300" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A301" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B301" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A302" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B302" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A303" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B303" s="4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A304" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B304" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A305" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B305" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A306" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B306" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A307" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B307" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A308" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B308" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A309" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B309" s="4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A310" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B310" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A311" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B311" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A312" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B312" s="4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A313" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B313" s="4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A314" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B314" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A315" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B315" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A316" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B316" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A317" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B317" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A318" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B318" s="4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A319" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B319" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A320" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B320" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A321" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B321" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A322" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B241" s="4" t="s">
+      <c r="B322" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A242" s="7" t="s">
+    <row r="323" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A323" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B242" s="4" t="s">
+      <c r="B323" s="4" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
+    <row r="324" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A324" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B243" s="4" t="s">
+      <c r="B324" s="4" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
+    <row r="325" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A325" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B244" s="4" t="s">
+      <c r="B325" s="4" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="2" t="s">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A326" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B245" s="4" t="s">
+      <c r="B326" s="4" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A327" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B246" s="4" t="s">
+      <c r="B327" s="4" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="2" t="s">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A328" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B247" s="4" t="s">
+      <c r="B328" s="4" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A248" s="2" t="s">
+    <row r="329" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A329" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B248" s="4" t="s">
+      <c r="B329" s="4" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
+    <row r="330" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A330" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B249" s="4" t="s">
+      <c r="B330" s="4" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
+    <row r="331" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A331" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B250" s="4" t="s">
+      <c r="B331" s="4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A251" s="7" t="s">
+    <row r="332" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A332" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="B251" s="6" t="s">
+      <c r="B332" s="6" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="252" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A252" s="2" t="s">
+    <row r="333" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A333" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B252" s="6" t="s">
+      <c r="B333" s="6" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A334" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B253" s="6" t="s">
+      <c r="B334" s="6" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="2" t="s">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A335" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B254" s="4" t="s">
+      <c r="B335" s="4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="2" t="s">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A336" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B255" s="4" t="s">
+      <c r="B336" s="4" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A256" s="2" t="s">
+    <row r="337" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A337" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B256" s="4" t="s">
+      <c r="B337" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A257" s="2" t="s">
+    <row r="338" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A338" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B257" s="4" t="s">
+      <c r="B338" s="4" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A258" s="7" t="s">
+    <row r="339" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+      <c r="A339" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B258" s="4" t="s">
+      <c r="B339" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A259" s="2" t="s">
+    <row r="340" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A340" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B259" s="4" t="s">
+      <c r="B340" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A260" s="7" t="s">
+    <row r="341" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A341" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B260" s="4" t="s">
+      <c r="B341" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="2" t="s">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A342" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B261" s="4" t="s">
+      <c r="B342" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A343" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B262" s="4" t="s">
+      <c r="B343" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A263" s="7" t="s">
+    <row r="344" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A344" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B344" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A345" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B345" s="4" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A346" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B346" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A347" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="B347" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A348" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B348" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A349" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B349" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A350" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B350" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A351" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B351" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A352" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B352" s="4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A353" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B353" s="4" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A354" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B354" s="4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A355" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B355" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A356" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B356" s="4" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A357" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B357" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A358" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B358" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A359" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B359" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A360" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B360" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A361" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B361" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A362" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="B263" s="4" t="s">
+      <c r="B362" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="2" t="s">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A363" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B264" s="4" t="s">
+      <c r="B363" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="2" t="s">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A364" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B265" s="4" t="s">
+      <c r="B364" s="4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="2" t="s">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A365" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B266" s="4" t="s">
+      <c r="B365" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2" t="s">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A366" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B267" s="4" t="s">
+      <c r="B366" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="2" t="s">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A367" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B268" s="4" t="s">
+      <c r="B367" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="2" t="s">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A368" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B269" s="4" t="s">
+      <c r="B368" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="2" t="s">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A369" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B270" s="4" t="s">
+      <c r="B369" s="4" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A370" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B271" s="4" t="s">
+      <c r="B370" s="4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="2" t="s">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A371" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B272" s="4" t="s">
+      <c r="B371" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="2" t="s">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A372" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B273" s="4" t="s">
+      <c r="B372" s="4" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="2" t="s">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A373" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B274" s="4" t="s">
+      <c r="B373" s="4" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="2" t="s">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A374" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B275" s="4" t="s">
+      <c r="B374" s="4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="2" t="s">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A375" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B276" s="4" t="s">
+      <c r="B375" s="4" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="2" t="s">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A376" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B277" s="4" t="s">
+      <c r="B376" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2" t="s">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A377" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B278" s="4" t="s">
+      <c r="B377" s="4" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="2" t="s">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A378" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B279" s="4" t="s">
+      <c r="B378" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="2" t="s">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A379" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B280" s="4" t="s">
+      <c r="B379" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="2" t="s">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A380" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B281" s="4" t="s">
+      <c r="B380" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="2" t="s">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A381" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B282" s="4" t="s">
+      <c r="B381" s="4" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="2" t="s">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A382" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B283" s="4" t="s">
+      <c r="B382" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="2" t="s">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A383" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B284" s="4" t="s">
+      <c r="B383" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="2" t="s">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A384" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B285" s="4" t="s">
+      <c r="B384" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="2" t="s">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A385" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B286" s="4" t="s">
+      <c r="B385" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="2" t="s">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A386" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B287" s="4" t="s">
+      <c r="B386" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="2" t="s">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A387" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B288" s="4" t="s">
+      <c r="B387" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="2" t="s">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A388" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B289" s="4" t="s">
+      <c r="B388" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="2" t="s">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A389" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B290" s="4" t="s">
+      <c r="B389" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="2" t="s">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A390" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B291" s="4" t="s">
+      <c r="B390" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="2" t="s">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A391" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B292" s="4" t="s">
+      <c r="B391" s="4" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="2" t="s">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A392" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B293" s="4" t="s">
+      <c r="B392" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="2" t="s">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A393" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B294" s="4" t="s">
+      <c r="B393" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="2" t="s">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A394" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B295" s="4" t="s">
+      <c r="B394" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="2" t="s">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A395" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B296" s="4" t="s">
+      <c r="B395" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="2" t="s">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A396" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B297" s="4" t="s">
+      <c r="B396" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="2" t="s">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A397" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B298" s="4" t="s">
+      <c r="B397" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A299" s="7" t="s">
+    <row r="398" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A398" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B299" s="4" t="s">
+      <c r="B398" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="2" t="s">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A399" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B300" s="4" t="s">
+      <c r="B399" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A301" s="7" t="s">
+    <row r="400" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A400" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B301" s="4" t="s">
+      <c r="B400" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="2" t="s">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A401" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B302" s="4" t="s">
+      <c r="B401" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="2" t="s">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A402" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B303" s="4" t="s">
+      <c r="B402" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A304" s="7" t="s">
+    <row r="403" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A403" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B304" s="4" t="s">
+      <c r="B403" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="2" t="s">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A404" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B305" s="4" t="s">
+      <c r="B404" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A306" s="7" t="s">
+    <row r="405" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A405" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B306" s="4" t="s">
+      <c r="B405" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="2" t="s">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A406" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B307" s="4" t="s">
+      <c r="B406" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="2" t="s">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A407" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B308" s="4" t="s">
+      <c r="B407" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A309" s="7" t="s">
+    <row r="408" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A408" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B309" s="4" t="s">
+      <c r="B408" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="2" t="s">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A409" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B310" s="4" t="s">
+      <c r="B409" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="2" t="s">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A410" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B311" s="4" t="s">
+      <c r="B410" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" s="2" t="s">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A411" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B312" s="4" t="s">
+      <c r="B411" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A313" s="7" t="s">
+    <row r="412" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A412" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B313" s="4" t="s">
+      <c r="B412" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A314" s="7" t="s">
+    <row r="413" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+      <c r="A413" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B314" s="4" t="s">
+      <c r="B413" s="4" t="s">
         <v>191</v>
       </c>
     </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A414"/>
+      <c r="B414"/>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A415"/>
+      <c r="B415"/>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A416"/>
+      <c r="B416"/>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A417"/>
+      <c r="B417"/>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A418"/>
+      <c r="B418"/>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A419"/>
+      <c r="B419"/>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A420"/>
+      <c r="B420"/>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A421"/>
+      <c r="B421"/>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A422"/>
+      <c r="B422"/>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A423"/>
+      <c r="B423"/>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A424"/>
+      <c r="B424"/>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A425"/>
+      <c r="B425"/>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A426"/>
+      <c r="B426"/>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A427"/>
+      <c r="B427"/>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A428"/>
+      <c r="B428"/>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A429"/>
+      <c r="B429"/>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A430"/>
+      <c r="B430"/>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A431"/>
+      <c r="B431"/>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A432"/>
+      <c r="B432"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:B320">
-    <sortCondition ref="A2:A320"/>
-    <sortCondition ref="B2:B320"/>
+  <sortState ref="A2:B449">
+    <sortCondition ref="A2:A449"/>
+    <sortCondition ref="B2:B449"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="4294967293" r:id="rId1"/>
@@ -3953,7 +5052,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3965,7 +5064,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementing unary operator & and completing code coverage.
</commit_message>
<xml_diff>
--- a/test/Templates.xlsx
+++ b/test/Templates.xlsx
@@ -1661,14 +1661,14 @@
   <dimension ref="A1:B432"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="A255" sqref="A255"/>
+      <selection activeCell="I247" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="151.83984375" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.83984375" style="2"/>
+    <col min="1" max="1" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="151.85546875" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
@@ -1727,7 +1727,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>63</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:2" ht="63.75" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>64</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>40</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>51</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>33</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>34</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>92</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="327.9" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:2" ht="378.75" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>89</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
+    <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>90</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
+    <row r="31" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>91</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>158</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="409.6" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>82</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>83</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="35" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>84</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:2" ht="48" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>85</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="93.9" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:2" ht="95.25" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>86</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="171.9" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:2" ht="189.75" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>87</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="171.9" x14ac:dyDescent="0.65">
+    <row r="39" spans="1:2" ht="189.75" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>88</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>76</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>76</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>72</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>72</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>72</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>72</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>70</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>18</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="50" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>53</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="51" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>141</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>141</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>141</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>141</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>75</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>206</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>206</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>206</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>206</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>206</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>206</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>218</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>218</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>218</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>218</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>218</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>212</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>212</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>212</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>212</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>212</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="72" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>94</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>45</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="74" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>353</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="75" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>353</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>353</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="77" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>69</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="78" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>69</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>202</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>202</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>202</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="82" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>258</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>258</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>258</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>258</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>258</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>258</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>258</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>258</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>258</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>258</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>258</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>258</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>258</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>258</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>258</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>258</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>258</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>258</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>258</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>258</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>258</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>258</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>258</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>258</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>258</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>258</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>258</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>258</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>258</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>258</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>258</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>258</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>258</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>258</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>258</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>258</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="118" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
         <v>30</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="119" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>30</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>30</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="121" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
         <v>303</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>303</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>303</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="124" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>303</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>303</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>303</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="127" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>303</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="128" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>303</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="129" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>303</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="130" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>303</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="131" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>303</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="132" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>303</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="133" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>303</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>303</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>303</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="136" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>303</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="137" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>303</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="138" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>303</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="139" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>102</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="140" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
         <v>104</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>104</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="142" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>242</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>242</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>242</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>242</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>242</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>242</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>242</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>242</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>242</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>242</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>242</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>242</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>242</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>242</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>242</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>242</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="158" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A158" s="7" t="s">
         <v>78</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>78</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>78</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>78</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>78</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="163" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A163" s="7" t="s">
         <v>32</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>32</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>32</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>32</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>32</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>32</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="169" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A169" s="7" t="s">
         <v>13</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="170" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
         <v>49</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="171" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
         <v>357</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>357</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="173" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>357</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>357</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>357</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>357</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="177" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>357</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="178" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>357</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="179" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>357</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="180" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>357</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="181" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>357</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>357</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>357</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>357</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="185" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>357</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="186" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>357</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="187" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
         <v>27</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>27</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="189" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A189" s="7" t="s">
         <v>79</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="190" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A190" s="7" t="s">
         <v>80</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>80</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>80</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>80</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>80</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>80</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>80</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="197" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>139</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="198" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>139</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="199" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
         <v>131</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>131</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="201" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>131</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="202" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
         <v>121</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="203" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A203" s="7" t="s">
         <v>138</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="204" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>138</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="205" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A205" s="7" t="s">
         <v>110</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>110</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="207" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>110</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>110</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="209" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A209" s="7" t="s">
         <v>25</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>25</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>25</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="212" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A212" s="7" t="s">
         <v>23</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="213" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
         <v>65</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>65</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>65</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="216" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A216" s="7" t="s">
         <v>97</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>97</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>97</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>97</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="47.1" x14ac:dyDescent="0.65">
+    <row r="220" spans="1:2" ht="48" x14ac:dyDescent="0.3">
       <c r="A220" s="7" t="s">
         <v>81</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="221" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A221" s="7" t="s">
         <v>35</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>35</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>35</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>35</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="225" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A225" s="7" t="s">
         <v>109</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="226" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A226" s="7" t="s">
         <v>93</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="227" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A227" s="7" t="s">
         <v>111</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>111</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>111</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>111</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>111</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>111</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="233" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A233" s="7" t="s">
         <v>223</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>223</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>223</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>223</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>223</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>223</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>223</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>223</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>223</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>223</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>223</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>223</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>223</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>223</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>223</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>223</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>223</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>223</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>223</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>223</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="253" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A253" s="7" t="s">
         <v>118</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>118</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="255" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A255" s="7" t="s">
         <v>417</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>417</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>417</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>417</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="259" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A259" s="7" t="s">
         <v>106</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>106</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="261" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A261" s="7" t="s">
         <v>77</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="262" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>77</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="263" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>77</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="264" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A264" s="7" t="s">
         <v>340</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>340</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>340</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>340</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>340</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="269" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="269" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A269" s="7" t="s">
         <v>377</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>377</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="271" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="271" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>377</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="272" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>377</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="273" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>377</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="78" x14ac:dyDescent="0.6">
+    <row r="274" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>377</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>377</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>377</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>377</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="278" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>377</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="279" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>377</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="171.6" x14ac:dyDescent="0.6">
+    <row r="280" spans="1:2" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>377</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="281" spans="1:2" ht="78" x14ac:dyDescent="0.6">
+    <row r="281" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>377</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="282" spans="1:2" ht="124.8" x14ac:dyDescent="0.6">
+    <row r="282" spans="1:2" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>377</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="283" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>377</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="284" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="284" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>377</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="285" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>377</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="286" spans="1:2" ht="78" x14ac:dyDescent="0.6">
+    <row r="286" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>377</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="287" spans="1:2" ht="156" x14ac:dyDescent="0.6">
+    <row r="287" spans="1:2" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>377</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>377</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="289" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>377</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="290" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>377</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>377</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="292" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>377</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="293" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>377</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="294" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>377</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="109.2" x14ac:dyDescent="0.6">
+    <row r="295" spans="1:2" ht="126" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>377</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="296" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>377</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="297" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>377</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="109.2" x14ac:dyDescent="0.6">
+    <row r="298" spans="1:2" ht="126" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>377</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="78" x14ac:dyDescent="0.6">
+    <row r="299" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>377</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="156" x14ac:dyDescent="0.6">
+    <row r="300" spans="1:2" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>377</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>377</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>377</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="303" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>377</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="304" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>377</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="305" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A305" s="7" t="s">
         <v>366</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>366</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="307" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>366</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="308" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>366</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>366</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>366</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="311" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="311" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A311" s="7" t="s">
         <v>369</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>369</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>369</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>369</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>369</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="316" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="316" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>369</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="317" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="317" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>369</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="318" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="318" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>369</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>369</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="320" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>369</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>369</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="322" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="322" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
         <v>369</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="323" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="323" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>369</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>369</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>369</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="326" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A326" s="7" t="s">
         <v>44</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="327" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A327" s="7" t="s">
         <v>296</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="328" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>296</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="329" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>296</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="330" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>296</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>296</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>296</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="333" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="333" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>296</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="334" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="334" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>296</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="335" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="335" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>296</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="336" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="336" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A336" s="7" t="s">
         <v>293</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="337" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="337" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>293</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>293</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>293</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>293</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="341" spans="1:2" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="341" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>293</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="342" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="342" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>293</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="343" spans="1:2" ht="31.5" x14ac:dyDescent="0.65">
+    <row r="343" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A343" s="7" t="s">
         <v>135</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="344" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>135</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="345" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A345" s="7" t="s">
         <v>21</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>21</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>21</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="348" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A348" s="7" t="s">
         <v>354</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="349" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>354</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>354</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="351" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A351" s="7" t="s">
         <v>341</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>341</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>341</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>341</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>341</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="356" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="356" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>341</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="357" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="357" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>341</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="358" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="358" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>341</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="359" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="359" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>341</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="360" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="360" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>341</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>341</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>341</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>341</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>341</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>341</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="366" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A366" s="7" t="s">
         <v>259</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>259</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>259</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>259</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>259</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>259</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>259</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>259</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>259</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>259</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>259</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>259</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>259</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>259</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>259</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>259</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>259</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>259</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
         <v>259</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>259</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>259</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>259</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>259</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>259</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
         <v>259</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
         <v>259</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
         <v>259</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>259</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
         <v>259</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>259</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>259</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>259</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
         <v>259</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
         <v>259</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>259</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>259</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="402" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="402" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A402" s="7" t="s">
         <v>58</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
         <v>58</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="404" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A404" s="7" t="s">
         <v>6</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>6</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
         <v>6</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="407" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A407" s="7" t="s">
         <v>10</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
         <v>10</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="409" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A409" s="7" t="s">
         <v>20</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
         <v>20</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
         <v>20</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="412" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A412" s="7" t="s">
         <v>2</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
         <v>2</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
         <v>2</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
         <v>2</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="416" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="416" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A416" s="7" t="s">
         <v>61</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="417" spans="1:2" ht="15.9" x14ac:dyDescent="0.65">
+    <row r="417" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A417" s="7" t="s">
         <v>140</v>
       </c>
@@ -5007,31 +5007,31 @@
         <v>191</v>
       </c>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418"/>
       <c r="B418"/>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427"/>
       <c r="B427"/>
     </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428"/>
       <c r="B428"/>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429"/>
       <c r="B429"/>
     </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430"/>
       <c r="B430"/>
     </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431"/>
       <c r="B431"/>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432"/>
       <c r="B432"/>
     </row>
@@ -5051,7 +5051,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5063,7 +5063,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Support of the legacy grammar.
</commit_message>
<xml_diff>
--- a/test/Templates.xlsx
+++ b/test/Templates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="430">
   <si>
     <t>LHS</t>
   </si>
@@ -1269,9 +1269,6 @@
     <t>variable_1 = ALLSHORTESTPATHS ( ( variable_1 :node_1 { parameter_1 } ) &lt;- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] -&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
   </si>
   <si>
-    <t>variable_1 = ALLSHORTESTPATHS ( ( variable_1 :node_1 { parameter_1 } ) &lt;- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] -&gt; ( variable_1 :node_1 { parameter_1 } ) ) , variable_1 = ALLSHORTESTPATHS ( ( variable_1 :node_1 { parameter_1 } ) &lt;- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] -&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
-  </si>
-  <si>
     <t>( variable_1 :node_1 { parameter_1 } ) &lt;- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] -&gt; ( variable_1 :node_1 { parameter_1 } )</t>
   </si>
   <si>
@@ -1303,13 +1300,19 @@
   </si>
   <si>
     <t>[ .. ]</t>
+  </si>
+  <si>
+    <t>variable_1 = ( ( variable_1 :node_1 { parameter_1 } ) &lt;- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] -&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
+  </si>
+  <si>
+    <t>variable_1 = ( ( variable_1 :node_1 { parameter_1 } ) &lt;- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] -&gt; ( variable_1 :node_1 { parameter_1 } ) ) , variable_1 = ( ( variable_1 :node_1 { parameter_1 } ) &lt;- [ variable_1 ?  : rel_type_1 | : rel_type_2 * 12 .. 34 { parameter_1 } ] -&gt; ( variable_1 :node_1 { parameter_1 } ) )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1330,8 +1333,28 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1350,6 +1373,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1360,10 +1388,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1373,13 +1402,18 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1681,13 +1715,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="B207" sqref="B207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="151.85546875" style="4" customWidth="1"/>
     <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
@@ -1701,7 +1735,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>127</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1709,15 +1743,15 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1765,79 +1799,79 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="63.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="8" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="8" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="8" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="8" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="8" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="8" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="8" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1853,7 +1887,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1861,7 +1895,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1877,7 +1911,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1885,7 +1919,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1901,7 +1935,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1909,7 +1943,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -1917,7 +1951,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="378.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1925,7 +1959,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1933,7 +1967,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>90</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1941,7 +1975,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1949,11 +1983,11 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -1965,7 +1999,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1973,7 +2007,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -1981,7 +2015,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="48" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -1989,7 +2023,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="95.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1997,7 +2031,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="189.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -2024,12 +2058,12 @@
       <c r="A42" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="189.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -2053,7 +2087,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>75</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -2069,7 +2103,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -2117,7 +2151,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -2125,7 +2159,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B55" s="4" t="s">
@@ -2133,7 +2167,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -2141,175 +2175,175 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="8" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="8" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="8" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="8" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="8" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="8" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="8" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="8" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="8" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="8" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="8" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="8" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="8" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="8" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="8" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="8" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="8" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="6" t="s">
         <v>93</v>
       </c>
       <c r="B78" s="4" t="s">
@@ -2317,7 +2351,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -2325,7 +2359,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="6" t="s">
         <v>338</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -2344,12 +2378,12 @@
       <c r="A82" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="5" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B83" s="4" t="s">
@@ -2365,319 +2399,319 @@
       </c>
     </row>
     <row r="85" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="8" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="8" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="8" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="8" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="8" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="8" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="8" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="8" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="8" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="8" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="8" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="8" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="8" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="8" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="8" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="8" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="8" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="8" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="8" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="8" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="8" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="8" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="8" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="8" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="8" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+      <c r="A110" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="8" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="8" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="8" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="8" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="8" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="8" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="8" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="8" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="8" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="8" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+      <c r="A121" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="8" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="8" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="8" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A124" s="7" t="s">
+      <c r="A124" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B124" s="4" t="s">
@@ -2701,7 +2735,7 @@
       </c>
     </row>
     <row r="127" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="6" t="s">
         <v>288</v>
       </c>
       <c r="B127" s="4" t="s">
@@ -2845,7 +2879,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A145" s="7" t="s">
+      <c r="A145" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B145" s="4" t="s">
@@ -2853,7 +2887,7 @@
       </c>
     </row>
     <row r="146" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A146" s="7" t="s">
+      <c r="A146" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B146" s="4" t="s">
@@ -2869,135 +2903,135 @@
       </c>
     </row>
     <row r="148" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A148" s="7" t="s">
+      <c r="A148" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="8" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
+      <c r="A149" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="8" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
+      <c r="A150" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B150" s="8" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
+      <c r="A151" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="8" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
+      <c r="A152" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B152" s="8" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
+      <c r="A153" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B153" s="8" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
+      <c r="A154" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="8" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
+      <c r="A155" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B155" s="8" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
+      <c r="A156" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B156" s="8" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
+      <c r="A157" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B157" s="8" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
+      <c r="A158" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B158" s="8" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="s">
+      <c r="A159" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B159" s="8" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
+      <c r="A160" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B160" s="8" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="s">
+      <c r="A161" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B161" s="8" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
+      <c r="A162" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B162" s="8" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
+      <c r="A163" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B163" s="8" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A164" s="7" t="s">
+      <c r="A164" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B164" s="4" t="s">
@@ -3037,7 +3071,7 @@
       </c>
     </row>
     <row r="169" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A169" s="7" t="s">
+      <c r="A169" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B169" s="4" t="s">
@@ -3085,7 +3119,7 @@
       </c>
     </row>
     <row r="175" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A175" s="7" t="s">
+      <c r="A175" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B175" s="4" t="s">
@@ -3093,7 +3127,7 @@
       </c>
     </row>
     <row r="176" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A176" s="7" t="s">
+      <c r="A176" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B176" s="4" t="s">
@@ -3101,7 +3135,7 @@
       </c>
     </row>
     <row r="177" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A177" s="7" t="s">
+      <c r="A177" s="6" t="s">
         <v>342</v>
       </c>
       <c r="B177" s="4" t="s">
@@ -3192,7 +3226,7 @@
       <c r="A188" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B188" s="6" t="s">
+      <c r="B188" s="5" t="s">
         <v>348</v>
       </c>
     </row>
@@ -3200,7 +3234,7 @@
       <c r="A189" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B189" s="6" t="s">
+      <c r="B189" s="5" t="s">
         <v>349</v>
       </c>
     </row>
@@ -3208,7 +3242,7 @@
       <c r="A190" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B190" s="6" t="s">
+      <c r="B190" s="5" t="s">
         <v>350</v>
       </c>
     </row>
@@ -3216,7 +3250,7 @@
       <c r="A191" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B191" s="6" t="s">
+      <c r="B191" s="5" t="s">
         <v>380</v>
       </c>
     </row>
@@ -3224,12 +3258,12 @@
       <c r="A192" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B192" s="6" t="s">
+      <c r="B192" s="5" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A193" s="7" t="s">
+      <c r="A193" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B193" s="4" t="s">
@@ -3245,7 +3279,7 @@
       </c>
     </row>
     <row r="195" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A195" s="7" t="s">
+      <c r="A195" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B195" s="4" t="s">
@@ -3253,7 +3287,7 @@
       </c>
     </row>
     <row r="196" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A196" s="7" t="s">
+      <c r="A196" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B196" s="4" t="s">
@@ -3309,11 +3343,11 @@
       </c>
     </row>
     <row r="203" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A203" s="7" t="s">
+      <c r="A203" s="6" t="s">
         <v>129</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="63" x14ac:dyDescent="0.25">
@@ -3321,11 +3355,11 @@
         <v>129</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A205" s="7" t="s">
+      <c r="A205" s="6" t="s">
         <v>124</v>
       </c>
       <c r="B205" s="4" t="s">
@@ -3345,19 +3379,19 @@
         <v>124</v>
       </c>
       <c r="B207" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A208" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B208" s="4" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A208" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B208" s="4" t="s">
-        <v>419</v>
-      </c>
-    </row>
     <row r="209" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A209" s="7" t="s">
+      <c r="A209" s="6" t="s">
         <v>128</v>
       </c>
       <c r="B209" s="4" t="s">
@@ -3373,23 +3407,23 @@
       </c>
     </row>
     <row r="211" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A211" s="7" t="s">
+      <c r="A211" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="B211" s="4" t="s">
+      <c r="B211" s="8" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
+      <c r="A212" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="B212" s="4" t="s">
+      <c r="B212" s="8" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A213" s="7" t="s">
+      <c r="A213" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B213" s="4" t="s">
@@ -3421,10 +3455,10 @@
       </c>
     </row>
     <row r="217" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A217" s="7" t="s">
+      <c r="A217" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B217" s="6" t="s">
+      <c r="B217" s="5" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3432,12 +3466,12 @@
       <c r="A218" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B218" s="6" t="s">
+      <c r="B218" s="5" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A219" s="7" t="s">
+      <c r="A219" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B219" s="4" t="s">
@@ -3445,7 +3479,7 @@
       </c>
     </row>
     <row r="220" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A220" s="7" t="s">
+      <c r="A220" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B220" s="4" t="s">
@@ -3469,7 +3503,7 @@
       </c>
     </row>
     <row r="223" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A223" s="7" t="s">
+      <c r="A223" s="6" t="s">
         <v>96</v>
       </c>
       <c r="B223" s="4" t="s">
@@ -3501,15 +3535,15 @@
       </c>
     </row>
     <row r="227" spans="1:2" ht="48" x14ac:dyDescent="0.3">
-      <c r="A227" s="7" t="s">
+      <c r="A227" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B227" s="4" t="s">
+      <c r="B227" s="8" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A228" s="7" t="s">
+      <c r="A228" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B228" s="4" t="s">
@@ -3541,15 +3575,15 @@
       </c>
     </row>
     <row r="232" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A232" s="7" t="s">
+      <c r="A232" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B232" s="4" t="s">
+      <c r="B232" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A233" s="7" t="s">
+      <c r="A233" s="6" t="s">
         <v>92</v>
       </c>
       <c r="B233" s="4" t="s">
@@ -3557,7 +3591,7 @@
       </c>
     </row>
     <row r="234" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A234" s="7" t="s">
+      <c r="A234" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B234" s="4" t="s">
@@ -3605,171 +3639,171 @@
       </c>
     </row>
     <row r="240" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A240" s="7" t="s">
+      <c r="A240" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B240" s="4" t="s">
+      <c r="B240" s="8" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="2" t="s">
+      <c r="A241" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B241" s="4" t="s">
+      <c r="B241" s="8" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="2" t="s">
+      <c r="A242" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B242" s="4" t="s">
+      <c r="B242" s="8" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
+      <c r="A243" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B243" s="4" t="s">
+      <c r="B243" s="8" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
+      <c r="A244" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B244" s="4" t="s">
+      <c r="B244" s="8" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="2" t="s">
+      <c r="A245" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B245" s="4" t="s">
+      <c r="B245" s="8" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
+      <c r="A246" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B246" s="4" t="s">
+      <c r="B246" s="8" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="2" t="s">
+      <c r="A247" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B247" s="4" t="s">
+      <c r="B247" s="8" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="2" t="s">
+      <c r="A248" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B248" s="4" t="s">
+      <c r="B248" s="8" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
+      <c r="A249" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B249" s="4" t="s">
+      <c r="B249" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
+      <c r="A250" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B250" s="4" t="s">
+      <c r="B250" s="8" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="2" t="s">
+      <c r="A251" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B251" s="4" t="s">
+      <c r="B251" s="8" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="2" t="s">
+      <c r="A252" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B252" s="4" t="s">
+      <c r="B252" s="8" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
+      <c r="A253" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B253" s="4" t="s">
+      <c r="B253" s="8" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="2" t="s">
+      <c r="A254" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B254" s="4" t="s">
+      <c r="B254" s="8" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="2" t="s">
+      <c r="A255" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B255" s="4" t="s">
+      <c r="B255" s="8" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="2" t="s">
+      <c r="A256" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B256" s="4" t="s">
+      <c r="B256" s="8" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="2" t="s">
+      <c r="A257" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B257" s="4" t="s">
+      <c r="B257" s="8" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="2" t="s">
+      <c r="A258" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B258" s="4" t="s">
+      <c r="B258" s="8" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="2" t="s">
+      <c r="A259" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B259" s="4" t="s">
+      <c r="B259" s="8" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A260" s="7" t="s">
+      <c r="A260" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -3777,35 +3811,35 @@
         <v>117</v>
       </c>
       <c r="B261" s="4" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A262" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="B262" s="8" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A262" s="7" t="s">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="B262" s="4" t="s">
+      <c r="B263" s="8" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="2" t="s">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="B263" s="4" t="s">
+      <c r="B264" s="8" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="B264" s="4" t="s">
-        <v>424</v>
-      </c>
-    </row>
     <row r="265" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A265" s="7" t="s">
+      <c r="A265" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B265" s="4" t="s">
@@ -3821,11 +3855,11 @@
       </c>
     </row>
     <row r="267" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A267" s="7" t="s">
+      <c r="A267" s="6" t="s">
         <v>76</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
@@ -3833,14 +3867,14 @@
         <v>76</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A269" s="7" t="s">
+      <c r="A269" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="B269" s="6" t="s">
+      <c r="B269" s="5" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3848,7 +3882,7 @@
       <c r="A270" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B270" s="6" t="s">
+      <c r="B270" s="5" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3856,7 +3890,7 @@
       <c r="A271" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B271" s="6" t="s">
+      <c r="B271" s="5" t="s">
         <v>313</v>
       </c>
     </row>
@@ -3877,7 +3911,7 @@
       </c>
     </row>
     <row r="274" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A274" s="7" t="s">
+      <c r="A274" s="6" t="s">
         <v>362</v>
       </c>
       <c r="B274" s="4" t="s">
@@ -4032,7 +4066,7 @@
       <c r="A293" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B293" s="6" t="s">
+      <c r="B293" s="5" t="s">
         <v>357</v>
       </c>
     </row>
@@ -4040,7 +4074,7 @@
       <c r="A294" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B294" s="6" t="s">
+      <c r="B294" s="5" t="s">
         <v>360</v>
       </c>
     </row>
@@ -4048,7 +4082,7 @@
       <c r="A295" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B295" s="6" t="s">
+      <c r="B295" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -4056,7 +4090,7 @@
       <c r="A296" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B296" s="6" t="s">
+      <c r="B296" s="5" t="s">
         <v>359</v>
       </c>
     </row>
@@ -4064,7 +4098,7 @@
       <c r="A297" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B297" s="6" t="s">
+      <c r="B297" s="5" t="s">
         <v>401</v>
       </c>
     </row>
@@ -4072,7 +4106,7 @@
       <c r="A298" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B298" s="6" t="s">
+      <c r="B298" s="5" t="s">
         <v>393</v>
       </c>
     </row>
@@ -4136,7 +4170,7 @@
       <c r="A306" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B306" s="6" t="s">
+      <c r="B306" s="5" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4144,7 +4178,7 @@
       <c r="A307" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B307" s="6" t="s">
+      <c r="B307" s="5" t="s">
         <v>353</v>
       </c>
     </row>
@@ -4152,7 +4186,7 @@
       <c r="A308" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B308" s="6" t="s">
+      <c r="B308" s="5" t="s">
         <v>394</v>
       </c>
     </row>
@@ -4160,12 +4194,12 @@
       <c r="A309" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B309" s="6" t="s">
+      <c r="B309" s="5" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A310" s="7" t="s">
+      <c r="A310" s="6" t="s">
         <v>351</v>
       </c>
       <c r="B310" s="4" t="s">
@@ -4200,7 +4234,7 @@
       <c r="A314" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B314" s="6" t="s">
+      <c r="B314" s="5" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4208,12 +4242,12 @@
       <c r="A315" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B315" s="6" t="s">
+      <c r="B315" s="5" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A316" s="7" t="s">
+      <c r="A316" s="6" t="s">
         <v>354</v>
       </c>
       <c r="B316" s="4" t="s">
@@ -4280,7 +4314,7 @@
       <c r="A324" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B324" s="6" t="s">
+      <c r="B324" s="5" t="s">
         <v>357</v>
       </c>
     </row>
@@ -4288,7 +4322,7 @@
       <c r="A325" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B325" s="6" t="s">
+      <c r="B325" s="5" t="s">
         <v>360</v>
       </c>
     </row>
@@ -4296,7 +4330,7 @@
       <c r="A326" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B326" s="6" t="s">
+      <c r="B326" s="5" t="s">
         <v>359</v>
       </c>
     </row>
@@ -4320,7 +4354,7 @@
       <c r="A329" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B329" s="6" t="s">
+      <c r="B329" s="5" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4328,12 +4362,12 @@
       <c r="A330" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B330" s="6" t="s">
+      <c r="B330" s="5" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A331" s="7" t="s">
+      <c r="A331" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B331" s="4" t="s">
@@ -4341,7 +4375,7 @@
       </c>
     </row>
     <row r="332" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A332" s="7" t="s">
+      <c r="A332" s="6" t="s">
         <v>281</v>
       </c>
       <c r="B332" s="4" t="s">
@@ -4413,10 +4447,10 @@
       </c>
     </row>
     <row r="341" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A341" s="7" t="s">
+      <c r="A341" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B341" s="6" t="s">
+      <c r="B341" s="5" t="s">
         <v>319</v>
       </c>
     </row>
@@ -4424,7 +4458,7 @@
       <c r="A342" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B342" s="6" t="s">
+      <c r="B342" s="5" t="s">
         <v>320</v>
       </c>
     </row>
@@ -4432,7 +4466,7 @@
       <c r="A343" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B343" s="6" t="s">
+      <c r="B343" s="5" t="s">
         <v>321</v>
       </c>
     </row>
@@ -4469,23 +4503,23 @@
       </c>
     </row>
     <row r="348" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A348" s="7" t="s">
+      <c r="A348" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B348" s="4" t="s">
-        <v>427</v>
+      <c r="B348" s="8" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A349" s="2" t="s">
+      <c r="A349" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B349" s="4" t="s">
+      <c r="B349" s="8" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A350" s="7" t="s">
+      <c r="A350" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B350" s="4" t="s">
@@ -4509,7 +4543,7 @@
       </c>
     </row>
     <row r="353" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A353" s="7" t="s">
+      <c r="A353" s="6" t="s">
         <v>339</v>
       </c>
       <c r="B353" s="4" t="s">
@@ -4528,12 +4562,12 @@
       <c r="A355" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B355" s="6" t="s">
+      <c r="B355" s="5" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A356" s="7" t="s">
+      <c r="A356" s="6" t="s">
         <v>326</v>
       </c>
       <c r="B356" s="4" t="s">
@@ -4616,7 +4650,7 @@
       <c r="A366" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B366" s="6" t="s">
+      <c r="B366" s="5" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4624,7 +4658,7 @@
       <c r="A367" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B367" s="6" t="s">
+      <c r="B367" s="5" t="s">
         <v>328</v>
       </c>
     </row>
@@ -4632,7 +4666,7 @@
       <c r="A368" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B368" s="6" t="s">
+      <c r="B368" s="5" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4640,7 +4674,7 @@
       <c r="A369" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B369" s="6" t="s">
+      <c r="B369" s="5" t="s">
         <v>335</v>
       </c>
     </row>
@@ -4648,300 +4682,300 @@
       <c r="A370" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B370" s="6" t="s">
+      <c r="B370" s="5" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A371" s="7" t="s">
+      <c r="A371" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="B371" s="4" t="s">
+      <c r="B371" s="8" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A372" s="2" t="s">
+      <c r="A372" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B372" s="4" t="s">
+      <c r="B372" s="8" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A373" s="2" t="s">
+      <c r="A373" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B373" s="4" t="s">
+      <c r="B373" s="8" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A374" s="2" t="s">
+      <c r="A374" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B374" s="4" t="s">
+      <c r="B374" s="8" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="2" t="s">
+      <c r="A375" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B375" s="4" t="s">
+      <c r="B375" s="8" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="2" t="s">
+      <c r="A376" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B376" s="4" t="s">
+      <c r="B376" s="8" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="2" t="s">
+      <c r="A377" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B377" s="4" t="s">
+      <c r="B377" s="8" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A378" s="2" t="s">
+      <c r="A378" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B378" s="4" t="s">
+      <c r="B378" s="8" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A379" s="2" t="s">
+      <c r="A379" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B379" s="4" t="s">
+      <c r="B379" s="8" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A380" s="2" t="s">
+      <c r="A380" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B380" s="4" t="s">
+      <c r="B380" s="8" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="2" t="s">
+      <c r="A381" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B381" s="4" t="s">
+      <c r="B381" s="8" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="2" t="s">
+      <c r="A382" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B382" s="4" t="s">
+      <c r="B382" s="8" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="2" t="s">
+      <c r="A383" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B383" s="4" t="s">
+      <c r="B383" s="8" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="2" t="s">
+      <c r="A384" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B384" s="4" t="s">
+      <c r="B384" s="8" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="2" t="s">
+      <c r="A385" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B385" s="4" t="s">
+      <c r="B385" s="8" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="2" t="s">
+      <c r="A386" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B386" s="4" t="s">
+      <c r="B386" s="8" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="2" t="s">
+      <c r="A387" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B387" s="4" t="s">
+      <c r="B387" s="8" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="2" t="s">
+      <c r="A388" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B388" s="4" t="s">
+      <c r="B388" s="8" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="2" t="s">
+      <c r="A389" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B389" s="4" t="s">
+      <c r="B389" s="8" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A390" s="2" t="s">
+      <c r="A390" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B390" s="4" t="s">
+      <c r="B390" s="8" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" s="2" t="s">
+      <c r="A391" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B391" s="4" t="s">
+      <c r="B391" s="8" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="2" t="s">
+      <c r="A392" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B392" s="4" t="s">
+      <c r="B392" s="8" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="2" t="s">
+      <c r="A393" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B393" s="4" t="s">
+      <c r="B393" s="8" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A394" s="2" t="s">
+      <c r="A394" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B394" s="4" t="s">
+      <c r="B394" s="8" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A395" s="2" t="s">
+      <c r="A395" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B395" s="4" t="s">
+      <c r="B395" s="8" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A396" s="2" t="s">
+      <c r="A396" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B396" s="4" t="s">
+      <c r="B396" s="8" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A397" s="2" t="s">
+      <c r="A397" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B397" s="4" t="s">
+      <c r="B397" s="8" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="2" t="s">
+      <c r="A398" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B398" s="4" t="s">
+      <c r="B398" s="8" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="2" t="s">
+      <c r="A399" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B399" s="4" t="s">
+      <c r="B399" s="8" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A400" s="2" t="s">
+      <c r="A400" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B400" s="4" t="s">
+      <c r="B400" s="8" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A401" s="2" t="s">
+      <c r="A401" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B401" s="4" t="s">
+      <c r="B401" s="8" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="2" t="s">
+      <c r="A402" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B402" s="4" t="s">
+      <c r="B402" s="8" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="2" t="s">
+      <c r="A403" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B403" s="4" t="s">
+      <c r="B403" s="8" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="2" t="s">
+      <c r="A404" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B404" s="4" t="s">
+      <c r="B404" s="8" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="2" t="s">
+      <c r="A405" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B405" s="4" t="s">
+      <c r="B405" s="8" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" s="2" t="s">
+      <c r="A406" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B406" s="4" t="s">
+      <c r="B406" s="8" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A407" s="7" t="s">
+      <c r="A407" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B407" s="4" t="s">
@@ -4957,7 +4991,7 @@
       </c>
     </row>
     <row r="409" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A409" s="7" t="s">
+      <c r="A409" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B409" s="4" t="s">
@@ -4981,7 +5015,7 @@
       </c>
     </row>
     <row r="412" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A412" s="7" t="s">
+      <c r="A412" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B412" s="4" t="s">
@@ -4997,7 +5031,7 @@
       </c>
     </row>
     <row r="414" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A414" s="7" t="s">
+      <c r="A414" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B414" s="4" t="s">
@@ -5021,7 +5055,7 @@
       </c>
     </row>
     <row r="417" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A417" s="7" t="s">
+      <c r="A417" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B417" s="4" t="s">
@@ -5053,7 +5087,7 @@
       </c>
     </row>
     <row r="421" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A421" s="7" t="s">
+      <c r="A421" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B421" s="4" t="s">
@@ -5061,7 +5095,7 @@
       </c>
     </row>
     <row r="422" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A422" s="7" t="s">
+      <c r="A422" s="6" t="s">
         <v>130</v>
       </c>
       <c r="B422" s="4" t="s">

</xml_diff>